<commit_message>
edit path and edit test case
</commit_message>
<xml_diff>
--- a/data/data_http.xlsx
+++ b/data/data_http.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20363"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1648EE-1A95-439B-A41C-D49E64AB24D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232A912B-C83D-47B6-9D91-CDD7F3BA021D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,36 +50,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{'email':'ktp0215926300','password':'test123','remember':0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'email':'ktp0215926300','password':'','remember':0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'email':'','password':'test123','remember':0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{'email':'ktp0215926300','password':'error123','remember':0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>success</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>email no null</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>passwd no null</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>passwd error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>密码不能为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户名不能为空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'email':'ktp0215926300','password':'test123','remember':0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'email':'','password':'test123','remember':0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'email':'ktp0215926300','password':'','remember':0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{'email':'ktp0215926300','password':'error123','remember':0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码错误, 你还可以尝试4次</t>
   </si>
 </sst>
 </file>
@@ -428,14 +427,14 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.25" customWidth="1"/>
     <col min="3" max="3" width="52.375" customWidth="1"/>
-    <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="4" max="4" width="29.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -463,10 +462,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -480,10 +479,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -497,10 +496,10 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -514,7 +513,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>

</xml_diff>